<commit_message>
just update to pom.xml
</commit_message>
<xml_diff>
--- a/src/main/resources/testData/demo.xlsx
+++ b/src/main/resources/testData/demo.xlsx
@@ -1,15 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28410"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bsingh5/git/excel-tutorial-with-dataDrivenFramework/src/main/resources/testData/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{D1671861-4565-4D18-A9F7-EA3E05824C6E}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16200" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14790" windowHeight="3360" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
@@ -19,6 +15,7 @@
     <sheet name="leadsData" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
+  <oleSize ref="A1:L8"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -315,8 +312,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="20" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -568,6 +565,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -835,23 +835,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="13.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="9.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="21">
       <c r="A1" s="5" t="s">
         <v>19</v>
       </c>
@@ -874,7 +874,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="21">
       <c r="A2" s="3" t="s">
         <v>25</v>
       </c>
@@ -897,7 +897,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="21">
       <c r="A3" s="3" t="s">
         <v>26</v>
       </c>
@@ -920,7 +920,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="21">
       <c r="A4" s="3" t="s">
         <v>27</v>
       </c>
@@ -943,7 +943,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="21">
       <c r="A5" s="3" t="s">
         <v>28</v>
       </c>
@@ -966,38 +966,38 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="21">
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
     </row>
-    <row r="8" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="21">
       <c r="B8" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="22" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="23.25">
       <c r="A1" s="7" t="s">
         <v>8</v>
       </c>
@@ -1008,7 +1008,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="23.25">
       <c r="A2" s="8" t="s">
         <v>15</v>
       </c>
@@ -1019,7 +1019,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="23.25">
       <c r="A3" s="8" t="s">
         <v>16</v>
       </c>
@@ -1030,7 +1030,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="23.25">
       <c r="A4" s="8" t="s">
         <v>17</v>
       </c>
@@ -1041,7 +1041,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="23.25">
       <c r="A5" s="8" t="s">
         <v>18</v>
       </c>
@@ -1050,7 +1050,7 @@
       </c>
       <c r="C5" s="9"/>
     </row>
-    <row r="6" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="23.25">
       <c r="A6" s="10"/>
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
@@ -1061,20 +1061,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:U20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="21"/>
   <cols>
-    <col min="1" max="1" width="21.5" style="31" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" style="31" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21">
       <c r="A1" s="29"/>
       <c r="B1" s="13" t="s">
         <v>46</v>
@@ -1086,7 +1086,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21">
       <c r="A2" s="27" t="s">
         <v>92</v>
       </c>
@@ -1100,7 +1100,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21">
       <c r="A3" s="29"/>
       <c r="B3" s="14" t="s">
         <v>2</v>
@@ -1112,7 +1112,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21">
       <c r="A4" s="29"/>
       <c r="B4" s="14" t="s">
         <v>4</v>
@@ -1124,7 +1124,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21">
       <c r="A5" s="29"/>
       <c r="B5" s="14" t="s">
         <v>6</v>
@@ -1136,7 +1136,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21">
       <c r="A6" s="29"/>
       <c r="B6" s="14" t="s">
         <v>49</v>
@@ -1148,7 +1148,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21">
       <c r="A7" s="27" t="s">
         <v>52</v>
       </c>
@@ -1156,10 +1156,10 @@
       <c r="C7" s="12"/>
       <c r="D7" s="12"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21">
       <c r="A8" s="28"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21">
       <c r="A9" s="30"/>
       <c r="B9" s="23" t="s">
         <v>46</v>
@@ -1222,7 +1222,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21">
       <c r="A10" s="13" t="s">
         <v>90</v>
       </c>
@@ -1287,7 +1287,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21">
       <c r="A11" s="30"/>
       <c r="B11" s="25" t="s">
         <v>47</v>
@@ -1350,7 +1350,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21">
       <c r="A12" s="30"/>
       <c r="B12" s="25" t="s">
         <v>47</v>
@@ -1413,7 +1413,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21">
       <c r="A13" s="13" t="s">
         <v>91</v>
       </c>
@@ -1438,7 +1438,7 @@
       <c r="T13" s="12"/>
       <c r="U13" s="12"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21">
       <c r="A15" s="30"/>
       <c r="B15" s="13" t="s">
         <v>46</v>
@@ -1450,7 +1450,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21">
       <c r="A16" s="27" t="s">
         <v>54</v>
       </c>
@@ -1464,7 +1464,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" s="30"/>
       <c r="B17" s="14" t="s">
         <v>2</v>
@@ -1476,7 +1476,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" s="30"/>
       <c r="B18" s="14" t="s">
         <v>4</v>
@@ -1488,7 +1488,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" s="30"/>
       <c r="B19" s="14" t="s">
         <v>6</v>
@@ -1500,7 +1500,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20" s="30" t="s">
         <v>51</v>
       </c>
@@ -1515,16 +1515,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="21">
       <c r="A1" s="13" t="s">
         <v>46</v>
       </c>
@@ -1535,7 +1535,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="21">
       <c r="A2" s="1" t="s">
         <v>47</v>
       </c>
@@ -1546,7 +1546,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="21">
       <c r="A3" s="1" t="s">
         <v>47</v>
       </c>
@@ -1563,30 +1563,30 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="27.5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" ht="15.75">
       <c r="A1" s="21" t="s">
         <v>46</v>
       </c>
@@ -1648,7 +1648,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" ht="15.75">
       <c r="A2" s="16" t="s">
         <v>47</v>
       </c>
@@ -1710,7 +1710,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" ht="15.75">
       <c r="A3" s="16" t="s">
         <v>47</v>
       </c>
@@ -1772,7 +1772,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" ht="15.75">
       <c r="A4" s="16" t="s">
         <v>47</v>
       </c>

</xml_diff>

<commit_message>
add createLeadTest to testNG.xml
</commit_message>
<xml_diff>
--- a/src/main/resources/testData/demo.xlsx
+++ b/src/main/resources/testData/demo.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{D1671861-4565-4D18-A9F7-EA3E05824C6E}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{006C7CC7-4DF3-4E0A-842D-B6E172DFF426}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14790" windowHeight="3360" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14790" windowHeight="3360" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
     <sheet name="leadsData" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
-  <oleSize ref="A1:L8"/>
+  <oleSize ref="A1:J9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -1518,7 +1518,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
@@ -1566,8 +1566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:T4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>

</xml_diff>